<commit_message>
Materiały do Lab 10 i Lab 11 - Teksturowanie postaci - Wykorzystanie palety - Proste Animacje
</commit_message>
<xml_diff>
--- a/2020-2021/Lab10/Zeszyt1.xlsx
+++ b/2020-2021/Lab10/Zeszyt1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dokumenty\Prowadzone Zajęcia\GrafikaKomputerowa\Materialy\GrafikaKomuterowa\2020-2021\Lab10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85326AB-1EFA-4AC7-A3DE-9D7CA124CD50}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D911BB0A-50E5-473D-AA6C-C2FC36ADA113}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{629B4876-2B97-4952-AFA0-1F793ED09969}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="24">
   <si>
     <t>v</t>
   </si>
@@ -101,14 +101,29 @@
   </si>
   <si>
     <t>Mapa</t>
+  </si>
+  <si>
+    <t>Plik OBJ</t>
+  </si>
+  <si>
+    <t>Pamięć karty graficznej</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -421,7 +436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -483,6 +498,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -942,10 +960,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A46EF3-B70C-4E81-AE4D-3892D67022D1}">
-  <dimension ref="I1:V19"/>
+  <dimension ref="I1:V20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+      <selection activeCell="T4" sqref="T4:V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -959,74 +977,68 @@
     <col min="20" max="22" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="9:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="9:22" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I2" s="10" t="s">
+    <row r="1" spans="9:22" x14ac:dyDescent="0.3">
+      <c r="I1" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="N1" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+    </row>
+    <row r="2" spans="9:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="9:22" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="4"/>
-      <c r="N2" s="10" t="s">
+      <c r="K3" s="3"/>
+      <c r="L3" s="4"/>
+      <c r="N3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="15" t="s">
+      <c r="O3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="15" t="s">
+      <c r="P3" s="3"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="S2" s="16"/>
-      <c r="T2" s="15" t="s">
+      <c r="S3" s="16"/>
+      <c r="T3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="U2" s="3"/>
-      <c r="V2" s="4"/>
-    </row>
-    <row r="3" spans="9:22" x14ac:dyDescent="0.3">
-      <c r="I3" s="11">
-        <v>1</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="N3" s="11">
-        <v>1</v>
-      </c>
-      <c r="O3" s="5"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="6"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="4"/>
     </row>
     <row r="4" spans="9:22" x14ac:dyDescent="0.3">
       <c r="I4" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="N4" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O4" s="5"/>
       <c r="P4" s="2"/>
@@ -1039,19 +1051,19 @@
     </row>
     <row r="5" spans="9:22" x14ac:dyDescent="0.3">
       <c r="I5" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="L5" s="6" t="s">
         <v>1</v>
       </c>
       <c r="N5" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O5" s="5"/>
       <c r="P5" s="2"/>
@@ -1062,179 +1074,209 @@
       <c r="U5" s="2"/>
       <c r="V5" s="6"/>
     </row>
-    <row r="6" spans="9:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I6" s="12">
+    <row r="6" spans="9:22" x14ac:dyDescent="0.3">
+      <c r="I6" s="11">
+        <v>3</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N6" s="11">
+        <v>3</v>
+      </c>
+      <c r="O6" s="5"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="6"/>
+    </row>
+    <row r="7" spans="9:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I7" s="12">
         <v>4</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="L6" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="N6" s="12">
+      <c r="L7" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="N7" s="12">
         <v>4</v>
       </c>
-      <c r="O6" s="7"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="18"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="8"/>
-      <c r="V6" s="9"/>
-    </row>
-    <row r="7" spans="9:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="9:22" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I8" s="22" t="s">
+      <c r="O7" s="7"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="18"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="9"/>
+    </row>
+    <row r="8" spans="9:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="9:22" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I9" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="15" t="s">
+      <c r="J9" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="K8" s="4"/>
-      <c r="O8" s="19" t="s">
+      <c r="K9" s="4"/>
+      <c r="O9" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="21"/>
-    </row>
-    <row r="9" spans="9:22" x14ac:dyDescent="0.3">
-      <c r="I9" s="24">
-        <v>1</v>
-      </c>
-      <c r="J9" s="5" t="s">
+      <c r="P9" s="20"/>
+      <c r="Q9" s="21"/>
+    </row>
+    <row r="10" spans="9:22" x14ac:dyDescent="0.3">
+      <c r="I10" s="24">
+        <v>1</v>
+      </c>
+      <c r="J10" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="O9" s="25"/>
-      <c r="P9" s="26"/>
-      <c r="Q9" s="27"/>
-    </row>
-    <row r="10" spans="9:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I10" s="24">
-        <v>2</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>6</v>
       </c>
       <c r="K10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="O10" s="28"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="30"/>
-    </row>
-    <row r="11" spans="9:22" x14ac:dyDescent="0.3">
+      <c r="O10" s="25">
+        <v>1</v>
+      </c>
+      <c r="P10" s="26"/>
+      <c r="Q10" s="27"/>
+    </row>
+    <row r="11" spans="9:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I11" s="24">
+        <v>2</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="O11" s="28"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="30"/>
+    </row>
+    <row r="12" spans="9:22" x14ac:dyDescent="0.3">
+      <c r="I12" s="24">
         <v>3</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K11" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="9:22" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I12" s="23">
+      <c r="K12" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="9:22" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I13" s="23">
         <v>4</v>
       </c>
-      <c r="J12" s="7" t="s">
+      <c r="J13" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="K12" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="9:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="9:22" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I14" s="22" t="s">
+      <c r="K13" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="9:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="9:22" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I15" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="J14" s="13" t="s">
+      <c r="J15" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="K14" s="3"/>
-      <c r="L14" s="4"/>
-      <c r="O14" s="19" t="s">
+      <c r="K15" s="3"/>
+      <c r="L15" s="4"/>
+      <c r="O15" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="P14" s="21"/>
-    </row>
-    <row r="15" spans="9:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I15" s="23">
-        <v>1</v>
-      </c>
-      <c r="J15" s="14" t="s">
+      <c r="P15" s="21"/>
+    </row>
+    <row r="16" spans="9:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I16" s="23">
+        <v>1</v>
+      </c>
+      <c r="J16" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="K15" s="8" t="s">
+      <c r="K16" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="L15" s="9" t="s">
+      <c r="L16" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="O15" s="5"/>
-      <c r="P15" s="6"/>
-    </row>
-    <row r="16" spans="9:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I16" s="1"/>
       <c r="O16" s="5"/>
       <c r="P16" s="6"/>
     </row>
-    <row r="17" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J17" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="K17" s="20"/>
-      <c r="L17" s="21"/>
+    <row r="17" spans="9:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I17" s="1"/>
       <c r="O17" s="5"/>
       <c r="P17" s="6"/>
     </row>
-    <row r="18" spans="10:16" x14ac:dyDescent="0.3">
-      <c r="J18" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="K18" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="L18" s="27" t="s">
-        <v>20</v>
-      </c>
+    <row r="18" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="J18" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="K18" s="20"/>
+      <c r="L18" s="21"/>
       <c r="O18" s="5"/>
       <c r="P18" s="6"/>
     </row>
-    <row r="19" spans="10:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J19" s="28" t="s">
+    <row r="19" spans="9:16" x14ac:dyDescent="0.3">
+      <c r="J19" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="K19" s="29" t="s">
+      <c r="K19" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="L19" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="O19" s="5"/>
+      <c r="P19" s="6"/>
+    </row>
+    <row r="20" spans="9:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J20" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="K20" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="L19" s="30" t="s">
+      <c r="L20" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="O19" s="7"/>
-      <c r="P19" s="9"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T2:V2"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="O2:Q2"/>
+  <mergeCells count="11">
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="T3:V3"/>
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="N1:V1"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="O3:Q3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>